<commit_message>
To resolvendo o metodo de converter ainda, mas vou dormir
</commit_message>
<xml_diff>
--- a/teste principal.xlsx
+++ b/teste principal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uer\Desktop\Autômatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{F3CB54DC-11FA-47D9-B21F-0A139AD8A193}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4063BF54-7B76-49A2-9C75-916567F5086B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="5970" xr2:uid="{FFD77D64-A23B-4C12-9BB4-86C55E0415DE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="9">
   <si>
     <t>q0</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>q1q2</t>
+  </si>
+  <si>
+    <t>q0q1q2</t>
   </si>
 </sst>
 </file>
@@ -400,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C50F1DF9-1BE1-4BAB-98BC-395A4DBF5C03}">
-  <dimension ref="B2:E13"/>
+  <dimension ref="B2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,6 +518,50 @@
         <v>5</v>
       </c>
     </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Seguinte, por enqto fica assim, dps vou tentar colocar maiis coisa pra ler o doente, do jeito q ta agr ta funcionando bem os automatos de tamanho consideravel
</commit_message>
<xml_diff>
--- a/teste principal.xlsx
+++ b/teste principal.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael\RiderProjects\automatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uer\Desktop\Autômatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F825BA14-B880-4D24-95AD-F2BB86FD0E07}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="5970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="5970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="13">
   <si>
     <t>q0</t>
   </si>
@@ -57,12 +59,18 @@
   </si>
   <si>
     <t>inicial</t>
+  </si>
+  <si>
+    <t>AFN</t>
+  </si>
+  <si>
+    <t>AFD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -407,11 +415,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,6 +501,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
@@ -531,21 +544,15 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="B15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -555,9 +562,6 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
       <c r="B17" t="s">
         <v>7</v>
       </c>
@@ -573,27 +577,27 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB7F9CE-AF7A-4DB5-A08A-38ECF2E4635B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
agr fechou, com tooltip e tudo
</commit_message>
<xml_diff>
--- a/teste principal.xlsx
+++ b/teste principal.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uer\Desktop\Autômatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318BEA83-40FB-4E43-B509-F534496433F9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088A5BF9-515E-4E08-99D2-F7ECC737AF92}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="5970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="5970" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="50">
   <si>
     <t>q0</t>
   </si>
@@ -142,7 +143,40 @@
     <t>q15q16q17q18q8q19q9q10q12</t>
   </si>
   <si>
-    <t>PORRA DEU CERTO</t>
+    <t>qf</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>q1,q2,q4</t>
+  </si>
+  <si>
+    <t>q0q1q2q4</t>
+  </si>
+  <si>
+    <t>q0q1q2q4qf</t>
+  </si>
+  <si>
+    <t>q0q1q2q4q3</t>
+  </si>
+  <si>
+    <t>q0q1q2q4q5</t>
+  </si>
+  <si>
+    <t>q0q1q2q4q3qf</t>
+  </si>
+  <si>
+    <t>q0q1q2q4q5q6</t>
+  </si>
+  <si>
+    <t>q0q1q2q4q5q6qf</t>
+  </si>
+  <si>
+    <t>CONVERTIDO &gt;&gt;</t>
+  </si>
+  <si>
+    <t>CONVERTIDO</t>
   </si>
 </sst>
 </file>
@@ -504,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E18"/>
+  <dimension ref="A2:E19"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,42 +666,47 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>10</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>8</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>9</v>
       </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
         <v>5</v>
       </c>
     </row>
@@ -680,12 +719,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB7F9CE-AF7A-4DB5-A08A-38ECF2E4635B}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
     <col min="6" max="6" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="45.42578125" customWidth="1"/>
@@ -763,6 +803,9 @@
       <c r="D5" t="s">
         <v>16</v>
       </c>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
       <c r="F5" t="s">
         <v>37</v>
       </c>
@@ -777,9 +820,7 @@
       <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
@@ -925,4 +966,205 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C104BDF9-D634-4ED1-BE86-3F55FD08FAA4}">
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>